<commit_message>
Add SO of sumo 0 in athlete 0
</commit_message>
<xml_diff>
--- a/docs/Planning.xlsx
+++ b/docs/Planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcelhacker/Documents/opensim-deadlift-techniques/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6963A1C-8E74-2F43-8D11-166F39BB8A82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A63B108-8105-8D4D-9A9F-92C58BF5124A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="1" xr2:uid="{D596EE47-F267-354E-8852-8744F315EF1A}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" xr2:uid="{D596EE47-F267-354E-8852-8744F315EF1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Athlete_0" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="112">
   <si>
     <t>Markerlist</t>
   </si>
@@ -879,8 +879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49C58917-876B-9749-A7DD-54E93015FBD7}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" x14ac:dyDescent="0.3"/>
@@ -1267,9 +1267,15 @@
       <c r="F20" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
+      <c r="G20" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="21" spans="1:9" ht="24" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
@@ -1401,7 +1407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5133B66-AA81-A54A-8537-83B40003C672}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>

</xml_diff>